<commit_message>
fix all modules bug
</commit_message>
<xml_diff>
--- a/data/modules.xlsx
+++ b/data/modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelinaswinburne/Documents/vca/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CDAA30-B7D4-0E45-BB1C-5BE49FB8D572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5716BE1F-897B-6346-8977-B59A1CC38805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="500" windowWidth="26600" windowHeight="15600" xr2:uid="{930DA7D1-8742-EF49-ABBE-E917A430AA45}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1107,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F8B334-3C81-6E43-BD52-3A93C4CB6FC7}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="88" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>

</xml_diff>